<commit_message>
update supp data legends
</commit_message>
<xml_diff>
--- a/SuppTables/SuppTable1.xlsx
+++ b/SuppTables/SuppTable1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eltehu-my.sharepoint.com/personal/orsolya_pipek_ttk_elte_hu/Documents/ELTE/VEO/recombinant_detection/supplementary/tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eltehu-my.sharepoint.com/personal/orsolya_pipek_ttk_elte_hu/Documents/ELTE/VEO/recombinant_detection/githubdesktop_laptop/SARSCoV2-coinf/SuppTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D23E5EC1-90DD-4615-A048-B8FDAC958D28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{D23E5EC1-90DD-4615-A048-B8FDAC958D28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD187601-E46B-4B33-947C-621BC7BFD65A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -326,8 +326,18 @@
     <t>PRJNA853723</t>
   </si>
   <si>
+    <t>PRJEB53987</t>
+  </si>
+  <si>
+    <t>PRJEB50429</t>
+  </si>
+  <si>
+    <t>co-infection
+prevalence (%)</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Supplementary Table 1. </t>
+      <t xml:space="preserve">Supplementary Data 1. </t>
     </r>
     <r>
       <rPr>
@@ -339,16 +349,6 @@
       </rPr>
       <t>Co-infection prevalence in different studies. Studies are listed in decreasing order based on the total number of their good-quality samples. Studies highlighted in grey had co-infection prevalence larger than 20%.</t>
     </r>
-  </si>
-  <si>
-    <t>PRJEB53987</t>
-  </si>
-  <si>
-    <t>PRJEB50429</t>
-  </si>
-  <si>
-    <t>co-infection
-prevalence (%)</t>
   </si>
 </sst>
 </file>
@@ -449,28 +449,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -692,7 +691,7 @@
   <dimension ref="A1:E99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -704,12 +703,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="A1" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -721,1338 +720,1338 @@
       <c r="C2" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>99</v>
+      <c r="D2" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3">
         <v>759</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3">
         <v>801761</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="7">
         <v>9.46666151134814E-2</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="8">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
         <v>277</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4">
         <v>233288</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="7">
         <v>0.118737354686053</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5">
         <v>190</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5">
         <v>135145</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="7">
         <v>0.14058973694920199</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6">
         <v>550</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6">
         <v>124402</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="7">
         <v>0.44211507853571402</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7">
         <v>1400</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7">
         <v>105805</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="7">
         <v>1.32318888521336</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8">
         <v>125</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8">
         <v>84200</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="7">
         <v>0.148456057007125</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9">
         <v>472</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9">
         <v>75477</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="7">
         <v>0.625356068736171</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10">
         <v>26</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10">
         <v>67197</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="7">
         <v>3.8692203520990502E-2</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11">
         <v>978</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11">
         <v>59459</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="7">
         <v>1.64483089187507</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12">
         <v>9</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12">
         <v>46180</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="7">
         <v>1.9488956258120398E-2</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13">
         <v>72</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13">
         <v>36546</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="7">
         <v>0.19701198489574701</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14">
         <v>20</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14">
         <v>28150</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="7">
         <v>7.1047957371225504E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15">
         <v>50</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15">
         <v>21217</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="7">
         <v>0.23566008389498899</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="A16" t="s">
         <v>85</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16">
         <v>22</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16">
         <v>18532</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="7">
         <v>0.11871357651629599</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17">
         <v>6</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17">
         <v>17879</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="7">
         <v>3.3558923877174303E-2</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="A18" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18">
         <v>1672</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18">
         <v>17184</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="7">
         <v>9.7299813780260695</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="A19" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19">
         <v>29</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19">
         <v>14872</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="7">
         <v>0.194997310381925</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+      <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20">
         <v>25</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20">
         <v>13594</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="7">
         <v>0.18390466382227399</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+      <c r="A21" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21">
         <v>8</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21">
         <v>13290</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="7">
         <v>6.0195635816403303E-2</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+      <c r="A22" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22">
         <v>12</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22">
         <v>12779</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="7">
         <v>9.3904061350653406E-2</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+      <c r="A23" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23">
         <v>2</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23">
         <v>12650</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="7">
         <v>1.5810276679841799E-2</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="A24" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24">
         <v>3</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24">
         <v>11162</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24" s="7">
         <v>2.68769037806844E-2</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="A25" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B25">
         <v>40</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25">
         <v>11136</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D25" s="7">
         <v>0.35919540229885</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="A26" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="8">
+      <c r="B26">
         <v>40</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26">
         <v>11007</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26" s="7">
         <v>0.36340510584173702</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+      <c r="A27" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B27">
         <v>3</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27">
         <v>9259</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D27" s="7">
         <v>3.2400907225402301E-2</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+      <c r="A28" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="8">
+      <c r="B28">
         <v>8</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28">
         <v>8286</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28" s="7">
         <v>9.6548394882934999E-2</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+      <c r="A29" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="8">
+      <c r="B29">
         <v>67</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29">
         <v>7698</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D29" s="7">
         <v>0.87035593660691002</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+      <c r="A30" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B30">
         <v>13</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30">
         <v>7648</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D30" s="7">
         <v>0.169979079497907</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+      <c r="A31" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="8">
+      <c r="B31">
         <v>6</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C31">
         <v>7589</v>
       </c>
-      <c r="D31" s="9">
+      <c r="D31" s="7">
         <v>7.9061799973645999E-2</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
+      <c r="A32" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="8">
+      <c r="B32">
         <v>97</v>
       </c>
-      <c r="C32" s="8">
+      <c r="C32">
         <v>7389</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D32" s="7">
         <v>1.3127622141020401</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+      <c r="A33" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="8">
+      <c r="B33">
         <v>67</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C33">
         <v>7352</v>
       </c>
-      <c r="D33" s="9">
+      <c r="D33" s="7">
         <v>0.91131664853101202</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
+      <c r="A34" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="8">
+      <c r="B34">
         <v>3</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C34">
         <v>6719</v>
       </c>
-      <c r="D34" s="9">
+      <c r="D34" s="7">
         <v>4.4649501413900797E-2</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
+      <c r="A35" t="s">
         <v>36</v>
       </c>
-      <c r="B35" s="8">
-        <v>1</v>
-      </c>
-      <c r="C35" s="8">
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
         <v>6562</v>
       </c>
-      <c r="D35" s="9">
+      <c r="D35" s="7">
         <v>1.52392563242913E-2</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+      <c r="A36" t="s">
         <v>23</v>
       </c>
-      <c r="B36" s="8">
-        <v>1</v>
-      </c>
-      <c r="C36" s="8">
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
         <v>6237</v>
       </c>
-      <c r="D36" s="9">
+      <c r="D36" s="7">
         <v>1.60333493666827E-2</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+      <c r="A37" t="s">
         <v>32</v>
       </c>
-      <c r="B37" s="8">
+      <c r="B37">
         <v>7</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C37">
         <v>6172</v>
       </c>
-      <c r="D37" s="9">
+      <c r="D37" s="7">
         <v>0.113415424497731</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
+      <c r="A38" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="8">
+      <c r="B38">
         <v>18</v>
       </c>
-      <c r="C38" s="8">
+      <c r="C38">
         <v>6169</v>
       </c>
-      <c r="D38" s="9">
+      <c r="D38" s="7">
         <v>0.29178148808558901</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
+      <c r="A39" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="8">
+      <c r="B39">
         <v>30</v>
       </c>
-      <c r="C39" s="8">
+      <c r="C39">
         <v>5763</v>
       </c>
-      <c r="D39" s="9">
+      <c r="D39" s="7">
         <v>0.52056220718375801</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
+      <c r="A40" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="8">
+      <c r="B40">
         <v>9</v>
       </c>
-      <c r="C40" s="8">
+      <c r="C40">
         <v>4829</v>
       </c>
-      <c r="D40" s="9">
+      <c r="D40" s="7">
         <v>0.18637399047421799</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
+      <c r="A41" t="s">
         <v>35</v>
       </c>
-      <c r="B41" s="8">
+      <c r="B41">
         <v>4</v>
       </c>
-      <c r="C41" s="8">
+      <c r="C41">
         <v>4786</v>
       </c>
-      <c r="D41" s="9">
+      <c r="D41" s="7">
         <v>8.3577099874634297E-2</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
+      <c r="A42" t="s">
         <v>40</v>
       </c>
-      <c r="B42" s="8">
+      <c r="B42">
         <v>5</v>
       </c>
-      <c r="C42" s="8">
+      <c r="C42">
         <v>4692</v>
       </c>
-      <c r="D42" s="9">
+      <c r="D42" s="7">
         <v>0.106564364876385</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
+      <c r="A43" t="s">
         <v>41</v>
       </c>
-      <c r="B43" s="8">
+      <c r="B43">
         <v>24</v>
       </c>
-      <c r="C43" s="8">
+      <c r="C43">
         <v>3635</v>
       </c>
-      <c r="D43" s="9">
+      <c r="D43" s="7">
         <v>0.66024759284731704</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
+      <c r="A44" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="8">
+      <c r="B44">
         <v>7</v>
       </c>
-      <c r="C44" s="8">
+      <c r="C44">
         <v>3089</v>
       </c>
-      <c r="D44" s="9">
+      <c r="D44" s="7">
         <v>0.226610553577209</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
+      <c r="A45" t="s">
         <v>24</v>
       </c>
-      <c r="B45" s="8">
+      <c r="B45">
         <v>14</v>
       </c>
-      <c r="C45" s="8">
+      <c r="C45">
         <v>2432</v>
       </c>
-      <c r="D45" s="9">
+      <c r="D45" s="7">
         <v>0.57565789473684204</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="s">
+      <c r="A46" t="s">
         <v>89</v>
       </c>
-      <c r="B46" s="8">
+      <c r="B46">
         <v>2</v>
       </c>
-      <c r="C46" s="8">
+      <c r="C46">
         <v>2151</v>
       </c>
-      <c r="D46" s="9">
+      <c r="D46" s="7">
         <v>9.2980009298000904E-2</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
+      <c r="A47" t="s">
         <v>44</v>
       </c>
-      <c r="B47" s="8">
+      <c r="B47">
         <v>10</v>
       </c>
-      <c r="C47" s="8">
+      <c r="C47">
         <v>2076</v>
       </c>
-      <c r="D47" s="9">
+      <c r="D47" s="7">
         <v>0.48169556840076999</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="s">
+      <c r="A48" t="s">
         <v>37</v>
       </c>
-      <c r="B48" s="8">
+      <c r="B48">
         <v>9</v>
       </c>
-      <c r="C48" s="8">
+      <c r="C48">
         <v>1767</v>
       </c>
-      <c r="D48" s="9">
+      <c r="D48" s="7">
         <v>0.50933786078098398</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="8" t="s">
+      <c r="A49" t="s">
         <v>43</v>
       </c>
-      <c r="B49" s="8">
+      <c r="B49">
         <v>6</v>
       </c>
-      <c r="C49" s="8">
+      <c r="C49">
         <v>1709</v>
       </c>
-      <c r="D49" s="9">
+      <c r="D49" s="7">
         <v>0.351082504388531</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
+      <c r="A50" t="s">
         <v>88</v>
       </c>
-      <c r="B50" s="8">
+      <c r="B50">
         <v>2</v>
       </c>
-      <c r="C50" s="8">
+      <c r="C50">
         <v>1608</v>
       </c>
-      <c r="D50" s="9">
+      <c r="D50" s="7">
         <v>0.124378109452736</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
+      <c r="A51" t="s">
         <v>48</v>
       </c>
-      <c r="B51" s="8">
+      <c r="B51">
         <v>13</v>
       </c>
-      <c r="C51" s="8">
+      <c r="C51">
         <v>1254</v>
       </c>
-      <c r="D51" s="9">
+      <c r="D51" s="7">
         <v>1.03668261562998</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
+      <c r="A52" t="s">
         <v>46</v>
       </c>
-      <c r="B52" s="8">
+      <c r="B52">
         <v>2</v>
       </c>
-      <c r="C52" s="8">
+      <c r="C52">
         <v>1195</v>
       </c>
-      <c r="D52" s="9">
+      <c r="D52" s="7">
         <v>0.167364016736401</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
+      <c r="A53" t="s">
         <v>47</v>
       </c>
-      <c r="B53" s="8">
+      <c r="B53">
         <v>108</v>
       </c>
-      <c r="C53" s="8">
+      <c r="C53">
         <v>1130</v>
       </c>
-      <c r="D53" s="9">
+      <c r="D53" s="7">
         <v>9.5575221238938006</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="8" t="s">
+      <c r="A54" t="s">
         <v>50</v>
       </c>
-      <c r="B54" s="8">
-        <v>1</v>
-      </c>
-      <c r="C54" s="8">
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
         <v>836</v>
       </c>
-      <c r="D54" s="9">
+      <c r="D54" s="7">
         <v>0.119617224880382</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="8" t="s">
+      <c r="A55" t="s">
         <v>53</v>
       </c>
-      <c r="B55" s="8">
+      <c r="B55">
         <v>16</v>
       </c>
-      <c r="C55" s="8">
+      <c r="C55">
         <v>797</v>
       </c>
-      <c r="D55" s="9">
+      <c r="D55" s="7">
         <v>2.0075282308657401</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="8" t="s">
+      <c r="A56" t="s">
         <v>51</v>
       </c>
-      <c r="B56" s="8">
+      <c r="B56">
         <v>12</v>
       </c>
-      <c r="C56" s="8">
+      <c r="C56">
         <v>782</v>
       </c>
-      <c r="D56" s="9">
+      <c r="D56" s="7">
         <v>1.53452685421994</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="8" t="s">
+      <c r="A57" t="s">
         <v>92</v>
       </c>
-      <c r="B57" s="8">
+      <c r="B57">
         <v>4</v>
       </c>
-      <c r="C57" s="8">
+      <c r="C57">
         <v>774</v>
       </c>
-      <c r="D57" s="9">
+      <c r="D57" s="7">
         <v>0.516795865633074</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="8" t="s">
+      <c r="A58" t="s">
         <v>52</v>
       </c>
-      <c r="B58" s="8">
+      <c r="B58">
         <v>9</v>
       </c>
-      <c r="C58" s="8">
+      <c r="C58">
         <v>773</v>
       </c>
-      <c r="D58" s="9">
+      <c r="D58" s="7">
         <v>1.16429495472186</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="8" t="s">
+      <c r="A59" t="s">
         <v>54</v>
       </c>
-      <c r="B59" s="8">
+      <c r="B59">
         <v>4</v>
       </c>
-      <c r="C59" s="8">
+      <c r="C59">
         <v>766</v>
       </c>
-      <c r="D59" s="9">
+      <c r="D59" s="7">
         <v>0.52219321148825004</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="8" t="s">
+      <c r="A60" t="s">
         <v>45</v>
       </c>
-      <c r="B60" s="8">
-        <v>1</v>
-      </c>
-      <c r="C60" s="8">
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60">
         <v>553</v>
       </c>
-      <c r="D60" s="9">
+      <c r="D60" s="7">
         <v>0.18083182640144599</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="8" t="s">
+      <c r="A61" t="s">
         <v>58</v>
       </c>
-      <c r="B61" s="8">
+      <c r="B61">
         <v>2</v>
       </c>
-      <c r="C61" s="8">
+      <c r="C61">
         <v>545</v>
       </c>
-      <c r="D61" s="9">
+      <c r="D61" s="7">
         <v>0.36697247706421998</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="8" t="s">
+      <c r="A62" t="s">
         <v>56</v>
       </c>
-      <c r="B62" s="8">
-        <v>1</v>
-      </c>
-      <c r="C62" s="8">
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
         <v>535</v>
       </c>
-      <c r="D62" s="9">
+      <c r="D62" s="7">
         <v>0.18691588785046701</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="8" t="s">
+      <c r="A63" t="s">
         <v>55</v>
       </c>
-      <c r="B63" s="8">
-        <v>1</v>
-      </c>
-      <c r="C63" s="8">
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63">
         <v>499</v>
       </c>
-      <c r="D63" s="9">
+      <c r="D63" s="7">
         <v>0.200400801603206</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="8" t="s">
+      <c r="A64" t="s">
+        <v>96</v>
+      </c>
+      <c r="B64">
+        <v>2</v>
+      </c>
+      <c r="C64">
+        <v>491</v>
+      </c>
+      <c r="D64" s="7">
+        <v>0.40733197556008099</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>59</v>
+      </c>
+      <c r="B65">
+        <v>6</v>
+      </c>
+      <c r="C65">
+        <v>414</v>
+      </c>
+      <c r="D65" s="7">
+        <v>1.4492753623188399</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>57</v>
+      </c>
+      <c r="B66">
+        <v>18</v>
+      </c>
+      <c r="C66">
+        <v>382</v>
+      </c>
+      <c r="D66" s="7">
+        <v>4.7120418848167498</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>60</v>
+      </c>
+      <c r="B67">
+        <v>3</v>
+      </c>
+      <c r="C67">
+        <v>373</v>
+      </c>
+      <c r="D67" s="7">
+        <v>0.80428954423592403</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>61</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68">
+        <v>322</v>
+      </c>
+      <c r="D68" s="7">
+        <v>0.31055900621117999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>62</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69">
+        <v>288</v>
+      </c>
+      <c r="D69" s="7">
+        <v>0.34722222222222199</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>63</v>
+      </c>
+      <c r="B70">
+        <v>5</v>
+      </c>
+      <c r="C70">
+        <v>254</v>
+      </c>
+      <c r="D70" s="7">
+        <v>1.9685039370078701</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>94</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71">
+        <v>253</v>
+      </c>
+      <c r="D71" s="7">
+        <v>0.39525691699604698</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>64</v>
+      </c>
+      <c r="B72">
+        <v>4</v>
+      </c>
+      <c r="C72">
+        <v>206</v>
+      </c>
+      <c r="D72" s="7">
+        <v>1.94174757281553</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B73" s="9">
+        <v>117</v>
+      </c>
+      <c r="C73" s="9">
+        <v>152</v>
+      </c>
+      <c r="D73" s="10">
+        <v>76.973684210526301</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>66</v>
+      </c>
+      <c r="B74">
+        <v>1</v>
+      </c>
+      <c r="C74">
+        <v>104</v>
+      </c>
+      <c r="D74" s="7">
+        <v>0.96153846153846101</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B75" s="9">
+        <v>44</v>
+      </c>
+      <c r="C75" s="9">
+        <v>101</v>
+      </c>
+      <c r="D75" s="10">
+        <v>43.564356435643496</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B76" s="9">
+        <v>82</v>
+      </c>
+      <c r="C76" s="9">
         <v>97</v>
       </c>
-      <c r="B64" s="8">
+      <c r="D76" s="10">
+        <v>84.536082474226802</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>68</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77">
+        <v>86</v>
+      </c>
+      <c r="D77" s="7">
+        <v>1.16279069767441</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>69</v>
+      </c>
+      <c r="B78">
+        <v>1</v>
+      </c>
+      <c r="C78">
+        <v>86</v>
+      </c>
+      <c r="D78" s="7">
+        <v>1.16279069767441</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>70</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="C79">
+        <v>83</v>
+      </c>
+      <c r="D79" s="7">
+        <v>1.2048192771084301</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>71</v>
+      </c>
+      <c r="B80">
         <v>2</v>
       </c>
-      <c r="C64" s="8">
-        <v>491</v>
-      </c>
-      <c r="D64" s="9">
-        <v>0.40733197556008099</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B65" s="8">
+      <c r="C80">
+        <v>82</v>
+      </c>
+      <c r="D80" s="7">
+        <v>2.4390243902439002</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>72</v>
+      </c>
+      <c r="B81">
+        <v>1</v>
+      </c>
+      <c r="C81">
+        <v>80</v>
+      </c>
+      <c r="D81" s="7">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>86</v>
+      </c>
+      <c r="B82">
+        <v>1</v>
+      </c>
+      <c r="C82">
+        <v>79</v>
+      </c>
+      <c r="D82" s="7">
+        <v>1.26582278481012</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>74</v>
+      </c>
+      <c r="B83">
+        <v>1</v>
+      </c>
+      <c r="C83">
+        <v>76</v>
+      </c>
+      <c r="D83" s="7">
+        <v>1.31578947368421</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>73</v>
+      </c>
+      <c r="B84">
+        <v>4</v>
+      </c>
+      <c r="C84">
+        <v>76</v>
+      </c>
+      <c r="D84" s="7">
+        <v>5.2631578947368398</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>75</v>
+      </c>
+      <c r="B85">
         <v>6</v>
       </c>
-      <c r="C65" s="8">
-        <v>414</v>
-      </c>
-      <c r="D65" s="9">
-        <v>1.4492753623188399</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B66" s="8">
-        <v>18</v>
-      </c>
-      <c r="C66" s="8">
-        <v>382</v>
-      </c>
-      <c r="D66" s="9">
-        <v>4.7120418848167498</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="8" t="s">
+      <c r="C85">
+        <v>75</v>
+      </c>
+      <c r="D85" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>76</v>
+      </c>
+      <c r="B86">
+        <v>1</v>
+      </c>
+      <c r="C86">
+        <v>73</v>
+      </c>
+      <c r="D86" s="7">
+        <v>1.3698630136986301</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>97</v>
+      </c>
+      <c r="B87">
+        <v>1</v>
+      </c>
+      <c r="C87">
+        <v>70</v>
+      </c>
+      <c r="D87" s="7">
+        <v>1.4285714285714199</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>77</v>
+      </c>
+      <c r="B88">
+        <v>1</v>
+      </c>
+      <c r="C88">
+        <v>64</v>
+      </c>
+      <c r="D88" s="7">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>87</v>
+      </c>
+      <c r="B89">
+        <v>3</v>
+      </c>
+      <c r="C89">
         <v>60</v>
       </c>
-      <c r="B67" s="8">
-        <v>3</v>
-      </c>
-      <c r="C67" s="8">
-        <v>373</v>
-      </c>
-      <c r="D67" s="9">
-        <v>0.80428954423592403</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B68" s="8">
-        <v>1</v>
-      </c>
-      <c r="C68" s="8">
-        <v>322</v>
-      </c>
-      <c r="D68" s="9">
-        <v>0.31055900621117999</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B69" s="8">
-        <v>1</v>
-      </c>
-      <c r="C69" s="8">
-        <v>288</v>
-      </c>
-      <c r="D69" s="9">
-        <v>0.34722222222222199</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B70" s="8">
+      <c r="D89" s="7">
         <v>5</v>
       </c>
-      <c r="C70" s="8">
-        <v>254</v>
-      </c>
-      <c r="D70" s="9">
-        <v>1.9685039370078701</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="B71" s="8">
-        <v>1</v>
-      </c>
-      <c r="C71" s="8">
-        <v>253</v>
-      </c>
-      <c r="D71" s="9">
-        <v>0.39525691699604698</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B72" s="8">
+    </row>
+    <row r="90" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>49</v>
+      </c>
+      <c r="B90">
+        <v>2</v>
+      </c>
+      <c r="C90">
+        <v>46</v>
+      </c>
+      <c r="D90" s="7">
+        <v>4.3478260869565197</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>91</v>
+      </c>
+      <c r="B91">
+        <v>1</v>
+      </c>
+      <c r="C91">
+        <v>12</v>
+      </c>
+      <c r="D91" s="7">
+        <v>8.3333333333333304</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B92" s="9">
+        <v>5</v>
+      </c>
+      <c r="C92" s="9">
+        <v>8</v>
+      </c>
+      <c r="D92" s="10">
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B93" s="9">
+        <v>5</v>
+      </c>
+      <c r="C93" s="9">
+        <v>7</v>
+      </c>
+      <c r="D93" s="10">
+        <v>71.428571428571402</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>79</v>
+      </c>
+      <c r="B94">
+        <v>1</v>
+      </c>
+      <c r="C94">
+        <v>6</v>
+      </c>
+      <c r="D94" s="7">
+        <v>16.6666666666666</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>78</v>
+      </c>
+      <c r="B95">
+        <v>1</v>
+      </c>
+      <c r="C95">
+        <v>6</v>
+      </c>
+      <c r="D95" s="7">
+        <v>16.6666666666666</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B96" s="9">
+        <v>1</v>
+      </c>
+      <c r="C96" s="9">
         <v>4</v>
       </c>
-      <c r="C72" s="8">
-        <v>206</v>
-      </c>
-      <c r="D72" s="9">
-        <v>1.94174757281553</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B73" s="11">
-        <v>117</v>
-      </c>
-      <c r="C73" s="11">
-        <v>152</v>
-      </c>
-      <c r="D73" s="12">
-        <v>76.973684210526301</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B74" s="8">
-        <v>1</v>
-      </c>
-      <c r="C74" s="8">
-        <v>104</v>
-      </c>
-      <c r="D74" s="9">
-        <v>0.96153846153846101</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B75" s="11">
-        <v>44</v>
-      </c>
-      <c r="C75" s="11">
-        <v>101</v>
-      </c>
-      <c r="D75" s="12">
-        <v>43.564356435643496</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B76" s="11">
-        <v>82</v>
-      </c>
-      <c r="C76" s="11">
-        <v>97</v>
-      </c>
-      <c r="D76" s="12">
-        <v>84.536082474226802</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B77" s="8">
-        <v>1</v>
-      </c>
-      <c r="C77" s="8">
-        <v>86</v>
-      </c>
-      <c r="D77" s="9">
-        <v>1.16279069767441</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="B78" s="8">
-        <v>1</v>
-      </c>
-      <c r="C78" s="8">
-        <v>86</v>
-      </c>
-      <c r="D78" s="9">
-        <v>1.16279069767441</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B79" s="8">
-        <v>1</v>
-      </c>
-      <c r="C79" s="8">
-        <v>83</v>
-      </c>
-      <c r="D79" s="9">
-        <v>1.2048192771084301</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="B80" s="8">
-        <v>2</v>
-      </c>
-      <c r="C80" s="8">
-        <v>82</v>
-      </c>
-      <c r="D80" s="9">
-        <v>2.4390243902439002</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B81" s="8">
-        <v>1</v>
-      </c>
-      <c r="C81" s="8">
-        <v>80</v>
-      </c>
-      <c r="D81" s="9">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="B82" s="8">
-        <v>1</v>
-      </c>
-      <c r="C82" s="8">
-        <v>79</v>
-      </c>
-      <c r="D82" s="9">
-        <v>1.26582278481012</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B83" s="8">
-        <v>1</v>
-      </c>
-      <c r="C83" s="8">
-        <v>76</v>
-      </c>
-      <c r="D83" s="9">
-        <v>1.31578947368421</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B84" s="8">
-        <v>4</v>
-      </c>
-      <c r="C84" s="8">
-        <v>76</v>
-      </c>
-      <c r="D84" s="9">
-        <v>5.2631578947368398</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="B85" s="8">
-        <v>6</v>
-      </c>
-      <c r="C85" s="8">
-        <v>75</v>
-      </c>
-      <c r="D85" s="9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B86" s="8">
-        <v>1</v>
-      </c>
-      <c r="C86" s="8">
-        <v>73</v>
-      </c>
-      <c r="D86" s="9">
-        <v>1.3698630136986301</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="B87" s="8">
-        <v>1</v>
-      </c>
-      <c r="C87" s="8">
-        <v>70</v>
-      </c>
-      <c r="D87" s="9">
-        <v>1.4285714285714199</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B88" s="8">
-        <v>1</v>
-      </c>
-      <c r="C88" s="8">
-        <v>64</v>
-      </c>
-      <c r="D88" s="9">
-        <v>1.5625</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="B89" s="8">
-        <v>3</v>
-      </c>
-      <c r="C89" s="8">
-        <v>60</v>
-      </c>
-      <c r="D89" s="9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B90" s="8">
-        <v>2</v>
-      </c>
-      <c r="C90" s="8">
-        <v>46</v>
-      </c>
-      <c r="D90" s="9">
-        <v>4.3478260869565197</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="B91" s="8">
-        <v>1</v>
-      </c>
-      <c r="C91" s="8">
-        <v>12</v>
-      </c>
-      <c r="D91" s="9">
-        <v>8.3333333333333304</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B92" s="11">
-        <v>5</v>
-      </c>
-      <c r="C92" s="11">
-        <v>8</v>
-      </c>
-      <c r="D92" s="12">
-        <v>62.5</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="B93" s="11">
-        <v>5</v>
-      </c>
-      <c r="C93" s="11">
-        <v>7</v>
-      </c>
-      <c r="D93" s="12">
-        <v>71.428571428571402</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B94" s="8">
-        <v>1</v>
-      </c>
-      <c r="C94" s="8">
-        <v>6</v>
-      </c>
-      <c r="D94" s="9">
-        <v>16.6666666666666</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B95" s="8">
-        <v>1</v>
-      </c>
-      <c r="C95" s="8">
-        <v>6</v>
-      </c>
-      <c r="D95" s="9">
-        <v>16.6666666666666</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B96" s="11">
-        <v>1</v>
-      </c>
-      <c r="C96" s="11">
-        <v>4</v>
-      </c>
-      <c r="D96" s="12">
+      <c r="D96" s="10">
         <v>25</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="11" t="s">
+      <c r="A97" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B97" s="11">
-        <v>1</v>
-      </c>
-      <c r="C97" s="11">
-        <v>1</v>
-      </c>
-      <c r="D97" s="12">
+      <c r="B97" s="9">
+        <v>1</v>
+      </c>
+      <c r="C97" s="9">
+        <v>1</v>
+      </c>
+      <c r="D97" s="10">
         <v>100</v>
       </c>
     </row>

</xml_diff>